<commit_message>
se suben nuevos perfiles para la sección de IM
</commit_message>
<xml_diff>
--- a/SAT-SDMA-7 Perfiles.xlsx
+++ b/SAT-SDMA-7 Perfiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raquell.martinez\Documents\AISolutions\analyzeCV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69CDD08A-CBA0-4BF8-B3B8-C2EF0B1E9327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2658ECC1-7A17-4441-A666-75F96C7D67DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{D74C329F-941D-40F9-B295-21746B646AD6}"/>
   </bookViews>
@@ -1785,7 +1785,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1849,6 +1849,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1922,7 +1934,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2086,6 +2098,12 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3241,7 +3259,7 @@
       <pane xSplit="7" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3433,7 +3451,7 @@
       </c>
     </row>
     <row r="3" spans="1:41" ht="90" x14ac:dyDescent="0.35">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="66" t="s">
         <v>66</v>
       </c>
       <c r="C3" s="21" t="s">
@@ -4033,7 +4051,7 @@
       </c>
     </row>
     <row r="8" spans="1:41" ht="140" x14ac:dyDescent="0.35">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="66" t="s">
         <v>55</v>
       </c>
       <c r="C8" s="21" t="s">
@@ -4153,7 +4171,7 @@
       </c>
     </row>
     <row r="9" spans="1:41" ht="140" x14ac:dyDescent="0.35">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="66" t="s">
         <v>57</v>
       </c>
       <c r="C9" s="21" t="s">
@@ -4745,7 +4763,7 @@
       </c>
     </row>
     <row r="14" spans="1:41" ht="140" x14ac:dyDescent="0.35">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="66" t="s">
         <v>60</v>
       </c>
       <c r="C14" s="21" t="s">
@@ -4865,7 +4883,7 @@
       </c>
     </row>
     <row r="15" spans="1:41" ht="140" x14ac:dyDescent="0.35">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="67" t="s">
         <v>59</v>
       </c>
       <c r="C15" s="21" t="s">
@@ -4986,7 +5004,7 @@
     </row>
     <row r="16" spans="1:41" ht="89" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="57"/>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="66" t="s">
         <v>64</v>
       </c>
       <c r="C16" s="21" t="s">
@@ -5107,7 +5125,7 @@
     </row>
     <row r="17" spans="1:41" ht="70" x14ac:dyDescent="0.35">
       <c r="A17" s="58"/>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="67" t="s">
         <v>62</v>
       </c>
       <c r="C17" s="21" t="s">
@@ -14569,6 +14587,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="882a8f42-f1f9-4ba8-a024-a9506b2a3f1b" xsi:nil="true"/>
@@ -14578,15 +14605,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14609,6 +14627,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2F9F198-AAB3-4743-83B7-70E545DDE86B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{784A4964-F218-48FA-B8A8-6EC1F8CC6785}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -14623,12 +14649,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2F9F198-AAB3-4743-83B7-70E545DDE86B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>